<commit_message>
fix: router and db
</commit_message>
<xml_diff>
--- a/server/db.xlsx
+++ b/server/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -52,7 +52,49 @@
     <t>transportadora cam newton</t>
   </si>
   <si>
-    <t>00000000000000</t>
+    <t>granja transportes</t>
+  </si>
+  <si>
+    <t>transportadora caina</t>
+  </si>
+  <si>
+    <t>transportadora stefany</t>
+  </si>
+  <si>
+    <t>transporte delivery</t>
+  </si>
+  <si>
+    <t>delivery</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>granja@transportes</t>
+  </si>
+  <si>
+    <t>caina@email</t>
+  </si>
+  <si>
+    <t>stefany@email</t>
+  </si>
+  <si>
+    <t>transporte@delivery</t>
+  </si>
+  <si>
+    <t>delivery@email</t>
   </si>
   <si>
     <t>RJ</t>
@@ -61,7 +103,34 @@
     <t>SP</t>
   </si>
   <si>
-    <t>21888888888</t>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>67999994444</t>
+  </si>
+  <si>
+    <t>11111111111</t>
+  </si>
+  <si>
+    <t>123123</t>
+  </si>
+  <si>
+    <t>123123123123</t>
+  </si>
+  <si>
+    <t>123123321321</t>
   </si>
 </sst>
 </file>
@@ -419,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G2">
         <v>21888888888</v>
@@ -488,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G3">
         <v>21888888888</v>
@@ -511,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>21888888888</v>
@@ -527,17 +596,17 @@
       <c r="C5">
         <v>100</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="G5">
+        <v>21888888888</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -550,17 +619,132 @@
       <c r="C6">
         <v>100</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <v>21888888888</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="G6" t="s">
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix on routes and client side finished with validations
</commit_message>
<xml_diff>
--- a/server/db.xlsx
+++ b/server/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -22,115 +22,34 @@
     <t>Nome</t>
   </si>
   <si>
+    <t>Estado</t>
+  </si>
+  <si>
     <t>Preco_km</t>
   </si>
   <si>
     <t>Email</t>
   </si>
   <si>
+    <t>Telefone</t>
+  </si>
+  <si>
     <t>Avaliacao</t>
   </si>
   <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Telefone</t>
-  </si>
-  <si>
-    <t>Dms Logistics</t>
-  </si>
-  <si>
-    <t>transPetro</t>
-  </si>
-  <si>
-    <t>transportadora saquarema</t>
-  </si>
-  <si>
-    <t>transportadora araruama</t>
-  </si>
-  <si>
-    <t>transportadora cam newton</t>
-  </si>
-  <si>
-    <t>granja transportes</t>
-  </si>
-  <si>
-    <t>transportadora caina</t>
-  </si>
-  <si>
-    <t>transportadora stefany</t>
-  </si>
-  <si>
-    <t>transporte delivery</t>
-  </si>
-  <si>
-    <t>delivery</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>231</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>111</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>AC</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>granja@transportes</t>
-  </si>
-  <si>
-    <t>caina@email</t>
-  </si>
-  <si>
-    <t>stefany@email</t>
-  </si>
-  <si>
-    <t>transporte@delivery</t>
-  </si>
-  <si>
-    <t>delivery@email</t>
-  </si>
-  <si>
-    <t>RJ</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>CE</t>
-  </si>
-  <si>
-    <t>ES</t>
-  </si>
-  <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>PE</t>
-  </si>
-  <si>
-    <t>67999994444</t>
+    <t>a@a</t>
   </si>
   <si>
     <t>11111111111</t>
-  </si>
-  <si>
-    <t>123123</t>
-  </si>
-  <si>
-    <t>123123123123</t>
-  </si>
-  <si>
-    <t>123123321321</t>
   </si>
 </sst>
 </file>
@@ -488,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -524,227 +443,20 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
         <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2">
-        <v>21888888888</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3">
-        <v>21888888888</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4">
-        <v>21888888888</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5">
-        <v>21888888888</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6">
-        <v>21888888888</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor to create script file
</commit_message>
<xml_diff>
--- a/server/db.xlsx
+++ b/server/db.xlsx
@@ -43,10 +43,10 @@
     <t>AC</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>a@a</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>a@email</t>
   </si>
   <si>
     <t>11111111111</t>

</xml_diff>